<commit_message>
UPDATE: "Diccionario de datos"
Versión para el diseño de BD
</commit_message>
<xml_diff>
--- a/clases - diccionario de datos.xlsx
+++ b/clases - diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\adsi\sexto\oscar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B647E278-5972-4B29-B4A5-EFD9324971E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D57827E-9E37-4D8D-907A-9BEABA0CCC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FF41D06-D61B-4223-A4A5-12A9AB68D76C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="893">
   <si>
     <t>Microservicio Autenticación</t>
   </si>
@@ -2915,6 +2915,22 @@
   </si>
   <si>
     <t>Calendario / fecha de hoy</t>
+  </si>
+  <si>
+    <r>
+      <t>API /</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sura.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3828,7 +3844,7 @@
   <dimension ref="B3:BB122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6058,7 +6074,7 @@
         <v>827</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>849</v>
+        <v>892</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="3" t="s">

</xml_diff>

<commit_message>
UPDATE: se crean los campos de laboratorio
</commit_message>
<xml_diff>
--- a/clases - diccionario de datos.xlsx
+++ b/clases - diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\adsi\sexto\oscar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D57827E-9E37-4D8D-907A-9BEABA0CCC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C03B835-6FEB-48B4-97DE-A7157CD5C3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FF41D06-D61B-4223-A4A5-12A9AB68D76C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="954">
   <si>
     <t>Microservicio Autenticación</t>
   </si>
@@ -2931,6 +2931,189 @@
       </rPr>
       <t xml:space="preserve"> Sura.</t>
     </r>
+  </si>
+  <si>
+    <t>Historia No</t>
+  </si>
+  <si>
+    <t>Numero de historia</t>
+  </si>
+  <si>
+    <t>Documetno Paciente</t>
+  </si>
+  <si>
+    <t>Fecha de generacion</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Rechazado</t>
+  </si>
+  <si>
+    <t>Aprobado con restricciones</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Aplazado</t>
+  </si>
+  <si>
+    <t>Microservicio Laboratorio</t>
+  </si>
+  <si>
+    <t>Hema</t>
+  </si>
+  <si>
+    <t>Glice</t>
+  </si>
+  <si>
+    <t>ColesTot</t>
+  </si>
+  <si>
+    <t>Coleshdl</t>
+  </si>
+  <si>
+    <t>Colesldl</t>
+  </si>
+  <si>
+    <t>Trigli</t>
+  </si>
+  <si>
+    <t>ParcOri</t>
+  </si>
+  <si>
+    <t>CulOri</t>
+  </si>
+  <si>
+    <t>Copro</t>
+  </si>
+  <si>
+    <t>FrotsisFar</t>
+  </si>
+  <si>
+    <t>CultiFar</t>
+  </si>
+  <si>
+    <t>Koh</t>
+  </si>
+  <si>
+    <t>Tsh</t>
+  </si>
+  <si>
+    <t>Creat</t>
+  </si>
+  <si>
+    <t>FuncHep</t>
+  </si>
+  <si>
+    <t>ProtinC</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>Ptt</t>
+  </si>
+  <si>
+    <t>AciUri</t>
+  </si>
+  <si>
+    <t>AntigPros</t>
+  </si>
+  <si>
+    <t>GasArte</t>
+  </si>
+  <si>
+    <t>Vdrl</t>
+  </si>
+  <si>
+    <t>Gravi</t>
+  </si>
+  <si>
+    <t>Obser1.lab</t>
+  </si>
+  <si>
+    <t>Obser2.lab</t>
+  </si>
+  <si>
+    <t>Cuadro Hematico</t>
+  </si>
+  <si>
+    <t>Glicemia</t>
+  </si>
+  <si>
+    <t>Colesterol total</t>
+  </si>
+  <si>
+    <t>Colesterol HDL</t>
+  </si>
+  <si>
+    <t>Colesterol LDL</t>
+  </si>
+  <si>
+    <t>Trigliceridos</t>
+  </si>
+  <si>
+    <t>Parcial deOrina</t>
+  </si>
+  <si>
+    <t>Cultivo de Orina</t>
+  </si>
+  <si>
+    <t>Corpologico</t>
+  </si>
+  <si>
+    <t>Frotis Faringeo</t>
+  </si>
+  <si>
+    <t>Cultivo Faringeo</t>
+  </si>
+  <si>
+    <t>KOH</t>
+  </si>
+  <si>
+    <t>Creatinina</t>
+  </si>
+  <si>
+    <t>Pruebas de funcon hepatica</t>
+  </si>
+  <si>
+    <t>Proteina C reactiva</t>
+  </si>
+  <si>
+    <t>Pt (tiempo de protombia)</t>
+  </si>
+  <si>
+    <t>Ptt(tiempo parcial de tromboplatina)</t>
+  </si>
+  <si>
+    <t>Acido Urico</t>
+  </si>
+  <si>
+    <t>Antigeno Prostatico</t>
+  </si>
+  <si>
+    <t>Gases Arteriales</t>
+  </si>
+  <si>
+    <t>Gravidez</t>
+  </si>
+  <si>
+    <t>Observaciones 1</t>
+  </si>
+  <si>
+    <t>Observaciones 2</t>
+  </si>
+  <si>
+    <t>Normal / Anormal</t>
+  </si>
+  <si>
+    <t>char(18)</t>
   </si>
 </sst>
 </file>
@@ -3218,7 +3401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3293,11 +3476,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3307,6 +3496,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3325,24 +3520,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3380,9 +3557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3398,6 +3572,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3405,6 +3600,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3508,23 +3712,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3841,10 +4028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFD759A-78F0-4F71-BCD0-F7C29157BD1F}">
-  <dimension ref="B3:BB122"/>
+  <dimension ref="B3:BJ130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AQ46" sqref="AQ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3878,257 +4065,283 @@
     <col min="37" max="37" width="34.7109375" customWidth="1"/>
     <col min="38" max="38" width="70.28515625" customWidth="1"/>
     <col min="39" max="40" width="34.7109375" customWidth="1"/>
-    <col min="42" max="44" width="31.42578125" customWidth="1"/>
-    <col min="45" max="45" width="46" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.85546875" customWidth="1"/>
-    <col min="49" max="49" width="32.5703125" customWidth="1"/>
-    <col min="50" max="50" width="33.5703125" customWidth="1"/>
-    <col min="51" max="51" width="32.5703125" customWidth="1"/>
-    <col min="52" max="52" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="31.42578125" customWidth="1"/>
+    <col min="53" max="53" width="46" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="36.85546875" customWidth="1"/>
+    <col min="57" max="57" width="32.5703125" customWidth="1"/>
+    <col min="58" max="58" width="33.5703125" customWidth="1"/>
+    <col min="59" max="59" width="32.5703125" customWidth="1"/>
+    <col min="60" max="60" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="46" t="s">
+    <row r="3" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="48"/>
-      <c r="V4" s="46" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="54"/>
+      <c r="V4" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="48"/>
-      <c r="AA4" s="46" t="s">
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="54"/>
+      <c r="AA4" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="48"/>
-      <c r="AF4" s="46" t="s">
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="53"/>
+      <c r="AD4" s="54"/>
+      <c r="AF4" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="47"/>
-      <c r="AI4" s="48"/>
-      <c r="AK4" s="46" t="s">
+      <c r="AG4" s="53"/>
+      <c r="AH4" s="53"/>
+      <c r="AI4" s="54"/>
+      <c r="AK4" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="48"/>
-      <c r="AP4" s="73" t="s">
+      <c r="AL4" s="53"/>
+      <c r="AM4" s="53"/>
+      <c r="AN4" s="54"/>
+      <c r="AP4" s="52" t="s">
+        <v>903</v>
+      </c>
+      <c r="AQ4" s="53"/>
+      <c r="AR4" s="53"/>
+      <c r="AS4" s="54"/>
+      <c r="AX4" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="75"/>
-      <c r="AU4" s="10" t="s">
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="81"/>
+      <c r="BC4" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="AW4" s="46" t="s">
+      <c r="BE4" s="52" t="s">
         <v>319</v>
       </c>
-      <c r="AX4" s="47"/>
-      <c r="AY4" s="47"/>
-      <c r="AZ4" s="48"/>
-      <c r="BB4" s="10" t="s">
+      <c r="BF4" s="53"/>
+      <c r="BG4" s="53"/>
+      <c r="BH4" s="54"/>
+      <c r="BJ4" s="10" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="5" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B6" s="71" t="s">
+    <row r="5" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B6" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="47" t="s">
         <v>347</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="71" t="s">
+      <c r="G6" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="47" t="s">
         <v>347</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="71" t="s">
+      <c r="L6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="47" t="s">
         <v>347</v>
       </c>
       <c r="P6" s="5"/>
-      <c r="Q6" s="49" t="s">
+      <c r="Q6" s="72" t="s">
         <v>790</v>
       </c>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="51"/>
-      <c r="V6" s="38" t="s">
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="74"/>
+      <c r="V6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="W6" s="38" t="s">
+      <c r="W6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="X6" s="38" t="s">
+      <c r="X6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="Y6" s="38" t="s">
+      <c r="Y6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="AA6" s="38" t="s">
+      <c r="AA6" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="AB6" s="38" t="s">
+      <c r="AB6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="AC6" s="38" t="s">
+      <c r="AC6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="AD6" s="38" t="s">
+      <c r="AD6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="AF6" s="38" t="s">
+      <c r="AF6" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="AG6" s="38" t="s">
+      <c r="AG6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="AH6" s="38" t="s">
+      <c r="AH6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="AI6" s="38" t="s">
+      <c r="AI6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="AK6" s="38" t="s">
+      <c r="AK6" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AL6" s="38" t="s">
+      <c r="AL6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="AM6" s="38" t="s">
+      <c r="AM6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="AN6" s="38" t="s">
+      <c r="AN6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="AP6" s="38" t="s">
+      <c r="AP6" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="AQ6" s="47" t="s">
+        <v>340</v>
+      </c>
+      <c r="AR6" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="AS6" s="47" t="s">
+        <v>347</v>
+      </c>
+      <c r="AX6" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="AQ6" s="38" t="s">
+      <c r="AY6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="AR6" s="38" t="s">
+      <c r="AZ6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="AS6" s="38" t="s">
+      <c r="BA6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="AU6" s="38" t="s">
+      <c r="BC6" s="47" t="s">
         <v>313</v>
       </c>
-      <c r="AW6" s="38" t="s">
+      <c r="BE6" s="47" t="s">
         <v>320</v>
       </c>
-      <c r="AX6" s="38" t="s">
+      <c r="BF6" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="AY6" s="38" t="s">
+      <c r="BG6" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="AZ6" s="38" t="s">
+      <c r="BH6" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="BB6" s="38" t="s">
+      <c r="BJ6" s="47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="72"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
+    <row r="7" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="71"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="54"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="39"/>
-      <c r="X7" s="39"/>
-      <c r="Y7" s="39"/>
-      <c r="AA7" s="39"/>
-      <c r="AB7" s="39"/>
-      <c r="AC7" s="39"/>
-      <c r="AD7" s="39"/>
-      <c r="AF7" s="39"/>
-      <c r="AG7" s="39"/>
-      <c r="AH7" s="39"/>
-      <c r="AI7" s="39"/>
-      <c r="AK7" s="39"/>
-      <c r="AL7" s="39"/>
-      <c r="AM7" s="39"/>
-      <c r="AN7" s="39"/>
-      <c r="AP7" s="39"/>
-      <c r="AQ7" s="39"/>
-      <c r="AR7" s="39"/>
-      <c r="AS7" s="39"/>
-      <c r="AU7" s="67"/>
-      <c r="AW7" s="39"/>
-      <c r="AX7" s="39"/>
-      <c r="AY7" s="39"/>
-      <c r="AZ7" s="39"/>
-      <c r="BB7" s="67"/>
-    </row>
-    <row r="8" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B8" s="112" t="s">
+      <c r="Q7" s="75"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="77"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="AA7" s="48"/>
+      <c r="AB7" s="48"/>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="48"/>
+      <c r="AF7" s="48"/>
+      <c r="AG7" s="48"/>
+      <c r="AH7" s="48"/>
+      <c r="AI7" s="48"/>
+      <c r="AK7" s="48"/>
+      <c r="AL7" s="48"/>
+      <c r="AM7" s="48"/>
+      <c r="AN7" s="48"/>
+      <c r="AP7" s="48"/>
+      <c r="AQ7" s="48"/>
+      <c r="AR7" s="78"/>
+      <c r="AS7" s="78"/>
+      <c r="AX7" s="48"/>
+      <c r="AY7" s="48"/>
+      <c r="AZ7" s="48"/>
+      <c r="BA7" s="48"/>
+      <c r="BC7" s="48"/>
+      <c r="BE7" s="48"/>
+      <c r="BF7" s="48"/>
+      <c r="BG7" s="48"/>
+      <c r="BH7" s="48"/>
+      <c r="BJ7" s="48"/>
+    </row>
+    <row r="8" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -4166,16 +4379,16 @@
         <v>821</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="Q8" s="38" t="s">
+      <c r="Q8" s="47" t="s">
         <v>790</v>
       </c>
-      <c r="R8" s="38" t="s">
+      <c r="R8" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="S8" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="T8" s="47" t="s">
         <v>347</v>
       </c>
       <c r="V8" s="2" t="s">
@@ -4227,34 +4440,46 @@
         <v>475</v>
       </c>
       <c r="AP8" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="AQ8" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="AR8" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS8" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX8" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="AQ8" s="2" t="s">
+      <c r="AY8" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AR8" s="7" t="s">
+      <c r="AZ8" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="AS8" s="7" t="s">
+      <c r="BA8" s="7" t="s">
         <v>751</v>
       </c>
-      <c r="AU8" s="2"/>
-      <c r="AW8" s="2" t="s">
+      <c r="BC8" s="2"/>
+      <c r="BE8" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="AX8" s="2" t="s">
+      <c r="BF8" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="AY8" s="2" t="s">
+      <c r="BG8" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="AZ8" s="32" t="s">
+      <c r="BH8" s="32" t="s">
         <v>771</v>
       </c>
-      <c r="BB8" s="2"/>
-    </row>
-    <row r="9" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="113" t="s">
+      <c r="BJ8" s="2"/>
+    </row>
+    <row r="9" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -4292,10 +4517,10 @@
         <v>466</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
       <c r="V9" s="3" t="s">
         <v>36</v>
       </c>
@@ -4345,34 +4570,46 @@
         <v>475</v>
       </c>
       <c r="AP9" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="AQ9" s="6" t="s">
+        <v>930</v>
+      </c>
+      <c r="AR9" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS9" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX9" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="AQ9" s="3" t="s">
+      <c r="AY9" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="AR9" s="6" t="s">
+      <c r="AZ9" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AS9" s="6" t="s">
+      <c r="BA9" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="AU9" s="3"/>
-      <c r="AW9" s="3" t="s">
+      <c r="BC9" s="3"/>
+      <c r="BE9" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AX9" s="3" t="s">
+      <c r="BF9" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="AY9" s="3" t="s">
+      <c r="BG9" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="AZ9" s="3" t="s">
+      <c r="BH9" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB9" s="3"/>
-    </row>
-    <row r="10" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B10" s="113" t="s">
+      <c r="BJ9" s="3"/>
+    </row>
+    <row r="10" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B10" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -4471,34 +4708,46 @@
         <v>475</v>
       </c>
       <c r="AP10" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="AQ10" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="AR10" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS10" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX10" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="AQ10" s="3" t="s">
+      <c r="AY10" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="AR10" s="6" t="s">
+      <c r="AZ10" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AS10" s="6" t="s">
+      <c r="BA10" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="AU10" s="3"/>
-      <c r="AW10" s="3" t="s">
+      <c r="BC10" s="3"/>
+      <c r="BE10" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="AX10" s="3" t="s">
+      <c r="BF10" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="AY10" s="3" t="s">
+      <c r="BG10" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="AZ10" s="3" t="s">
+      <c r="BH10" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB10" s="3"/>
-    </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B11" s="113" t="s">
+      <c r="BJ10" s="3"/>
+    </row>
+    <row r="11" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B11" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -4597,34 +4846,46 @@
         <v>475</v>
       </c>
       <c r="AP11" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="AQ11" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="AR11" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS11" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX11" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="AQ11" s="3" t="s">
+      <c r="AY11" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="AR11" s="6" t="s">
+      <c r="AZ11" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AS11" s="6" t="s">
+      <c r="BA11" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="AU11" s="3"/>
-      <c r="AW11" s="3" t="s">
+      <c r="BC11" s="3"/>
+      <c r="BE11" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="AX11" s="6" t="s">
+      <c r="BF11" s="6" t="s">
         <v>755</v>
       </c>
-      <c r="AY11" s="3" t="s">
+      <c r="BG11" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="AZ11" s="3" t="s">
+      <c r="BH11" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB11" s="3"/>
-    </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B12" s="113" t="s">
+      <c r="BJ11" s="3"/>
+    </row>
+    <row r="12" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B12" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -4723,34 +4984,46 @@
         <v>475</v>
       </c>
       <c r="AP12" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="AQ12" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS12" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX12" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="AQ12" s="3" t="s">
+      <c r="AY12" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="AR12" s="6" t="s">
+      <c r="AZ12" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="AS12" s="6" t="s">
+      <c r="BA12" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AU12" s="3"/>
-      <c r="AW12" s="3" t="s">
+      <c r="BC12" s="3"/>
+      <c r="BE12" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="AX12" s="6" t="s">
+      <c r="BF12" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="AY12" s="3" t="s">
+      <c r="BG12" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="AZ12" s="3" t="s">
+      <c r="BH12" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB12" s="3"/>
-    </row>
-    <row r="13" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B13" s="113" t="s">
+      <c r="BJ12" s="3"/>
+    </row>
+    <row r="13" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B13" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -4759,7 +5032,7 @@
       <c r="D13" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="E13" s="110">
+      <c r="E13" s="38">
         <v>0</v>
       </c>
       <c r="F13" s="1"/>
@@ -4772,7 +5045,7 @@
       <c r="I13" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="J13" s="110">
+      <c r="J13" s="38">
         <v>0</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -4784,7 +5057,7 @@
       <c r="N13" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="O13" s="110">
+      <c r="O13" s="38">
         <v>0</v>
       </c>
       <c r="P13" s="1"/>
@@ -4849,34 +5122,46 @@
         <v>475</v>
       </c>
       <c r="AP13" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="AQ13" s="6" t="s">
+        <v>934</v>
+      </c>
+      <c r="AR13" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS13" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX13" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="AQ13" s="3" t="s">
+      <c r="AY13" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="AR13" s="6" t="s">
+      <c r="AZ13" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="AS13" s="6" t="s">
+      <c r="BA13" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="AU13" s="3"/>
-      <c r="AW13" s="3" t="s">
+      <c r="BC13" s="3"/>
+      <c r="BE13" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="AX13" s="6" t="s">
+      <c r="BF13" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="AY13" s="3" t="s">
+      <c r="BG13" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="AZ13" s="3" t="s">
+      <c r="BH13" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB13" s="3"/>
-    </row>
-    <row r="14" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="113" t="s">
+      <c r="BJ13" s="3"/>
+    </row>
+    <row r="14" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="41" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -4975,34 +5260,46 @@
         <v>475</v>
       </c>
       <c r="AP14" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="AQ14" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="AR14" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS14" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX14" s="3" t="s">
         <v>749</v>
       </c>
-      <c r="AQ14" s="3" t="s">
+      <c r="AY14" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="AR14" s="6" t="s">
+      <c r="AZ14" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="AS14" s="6" t="s">
+      <c r="BA14" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AU14" s="3"/>
-      <c r="AW14" s="3" t="s">
+      <c r="BC14" s="3"/>
+      <c r="BE14" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="AX14" s="6" t="s">
+      <c r="BF14" s="6" t="s">
         <v>759</v>
       </c>
-      <c r="AY14" s="3" t="s">
+      <c r="BG14" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="AZ14" s="3" t="s">
+      <c r="BH14" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB14" s="3"/>
-    </row>
-    <row r="15" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="113" t="s">
+      <c r="BJ14" s="3"/>
+    </row>
+    <row r="15" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -5093,34 +5390,46 @@
         <v>475</v>
       </c>
       <c r="AP15" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="AQ15" s="6" t="s">
+        <v>936</v>
+      </c>
+      <c r="AR15" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS15" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX15" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="AQ15" s="3" t="s">
+      <c r="AY15" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="AR15" s="6" t="s">
+      <c r="AZ15" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="AS15" s="6" t="s">
+      <c r="BA15" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AU15" s="3"/>
-      <c r="AW15" s="3" t="s">
+      <c r="BC15" s="3"/>
+      <c r="BE15" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="AX15" s="6" t="s">
+      <c r="BF15" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="AY15" s="3" t="s">
+      <c r="BG15" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="AZ15" s="3" t="s">
+      <c r="BH15" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB15" s="3"/>
-    </row>
-    <row r="16" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B16" s="113" t="s">
+      <c r="BJ15" s="3"/>
+    </row>
+    <row r="16" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B16" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -5210,33 +5519,45 @@
       <c r="AN16" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP16" s="68" t="s">
+      <c r="AP16" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="AQ16" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="AR16" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS16" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX16" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="AQ16" s="69"/>
-      <c r="AR16" s="69"/>
-      <c r="AS16" s="70"/>
-      <c r="AU16" s="7" t="s">
+      <c r="AY16" s="68"/>
+      <c r="AZ16" s="68"/>
+      <c r="BA16" s="69"/>
+      <c r="BC16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AW16" s="3" t="s">
+      <c r="BE16" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="AX16" s="6" t="s">
+      <c r="BF16" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="AY16" s="3" t="s">
+      <c r="BG16" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="AZ16" s="3" t="s">
+      <c r="BH16" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB16" s="7" t="s">
+      <c r="BJ16" s="7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B17" s="113" t="s">
+    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B17" s="41" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -5326,33 +5647,45 @@
       <c r="AN17" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP17" s="40" t="s">
+      <c r="AP17" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="AQ17" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="AR17" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS17" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX17" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="AQ17" s="41"/>
-      <c r="AR17" s="41"/>
-      <c r="AS17" s="42"/>
-      <c r="AU17" s="6" t="s">
+      <c r="AY17" s="45"/>
+      <c r="AZ17" s="45"/>
+      <c r="BA17" s="46"/>
+      <c r="BC17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AW17" s="3" t="s">
+      <c r="BE17" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="AX17" s="6" t="s">
+      <c r="BF17" s="6" t="s">
         <v>762</v>
       </c>
-      <c r="AY17" s="3" t="s">
+      <c r="BG17" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="AZ17" s="3" t="s">
+      <c r="BH17" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB17" s="6" t="s">
+      <c r="BJ17" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="113" t="s">
+    <row r="18" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -5444,33 +5777,45 @@
       <c r="AN18" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP18" s="40" t="s">
+      <c r="AP18" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="AQ18" s="6" t="s">
+        <v>939</v>
+      </c>
+      <c r="AR18" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS18" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX18" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="AQ18" s="41"/>
-      <c r="AR18" s="41"/>
-      <c r="AS18" s="42"/>
-      <c r="AU18" s="6" t="s">
+      <c r="AY18" s="45"/>
+      <c r="AZ18" s="45"/>
+      <c r="BA18" s="46"/>
+      <c r="BC18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AW18" s="3" t="s">
+      <c r="BE18" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="AX18" s="6" t="s">
+      <c r="BF18" s="6" t="s">
         <v>763</v>
       </c>
-      <c r="AY18" s="3" t="s">
+      <c r="BG18" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="AZ18" s="3" t="s">
+      <c r="BH18" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="BB18" s="6" t="s">
+      <c r="BJ18" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B19" s="113" t="s">
+    <row r="19" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B19" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -5556,33 +5901,45 @@
       <c r="AN19" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP19" s="40" t="s">
+      <c r="AP19" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="AQ19" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="AR19" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS19" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX19" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="AQ19" s="41"/>
-      <c r="AR19" s="41"/>
-      <c r="AS19" s="42"/>
-      <c r="AU19" s="3" t="s">
+      <c r="AY19" s="45"/>
+      <c r="AZ19" s="45"/>
+      <c r="BA19" s="46"/>
+      <c r="BC19" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="AW19" s="3" t="s">
+      <c r="BE19" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="AX19" s="6" t="s">
+      <c r="BF19" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="AY19" s="3" t="s">
+      <c r="BG19" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="AZ19" s="30" t="s">
+      <c r="BH19" s="30" t="s">
         <v>776</v>
       </c>
-      <c r="BB19" s="34" t="s">
+      <c r="BJ19" s="34" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B20" s="113"/>
+    <row r="20" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B20" s="41"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -5644,33 +6001,45 @@
       <c r="AN20" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP20" s="40" t="s">
+      <c r="AP20" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="AQ20" s="6" t="s">
+        <v>916</v>
+      </c>
+      <c r="AR20" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS20" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX20" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="AQ20" s="41"/>
-      <c r="AR20" s="41"/>
-      <c r="AS20" s="42"/>
-      <c r="AU20" s="3" t="s">
+      <c r="AY20" s="45"/>
+      <c r="AZ20" s="45"/>
+      <c r="BA20" s="46"/>
+      <c r="BC20" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="AW20" s="3" t="s">
+      <c r="BE20" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="AX20" s="6" t="s">
+      <c r="BF20" s="6" t="s">
         <v>765</v>
       </c>
-      <c r="AY20" s="3" t="s">
+      <c r="BG20" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="AZ20" s="6" t="s">
+      <c r="BH20" s="6" t="s">
         <v>777</v>
       </c>
-      <c r="BB20" s="3" t="s">
+      <c r="BJ20" s="3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B21" s="113" t="s">
+    <row r="21" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B21" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -5700,7 +6069,7 @@
       <c r="N21" s="6" t="s">
         <v>845</v>
       </c>
-      <c r="O21" s="110">
+      <c r="O21" s="38">
         <v>0</v>
       </c>
       <c r="P21" s="1"/>
@@ -5752,33 +6121,45 @@
       <c r="AN21" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP21" s="40" t="s">
+      <c r="AP21" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="AQ21" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="AR21" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS21" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX21" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AQ21" s="41"/>
-      <c r="AR21" s="41"/>
-      <c r="AS21" s="42"/>
-      <c r="AU21" s="3" t="s">
+      <c r="AY21" s="45"/>
+      <c r="AZ21" s="45"/>
+      <c r="BA21" s="46"/>
+      <c r="BC21" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="AW21" s="3" t="s">
+      <c r="BE21" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="AX21" s="6" t="s">
+      <c r="BF21" s="6" t="s">
         <v>768</v>
       </c>
-      <c r="AY21" s="6" t="s">
+      <c r="BG21" s="6" t="s">
         <v>773</v>
       </c>
-      <c r="AZ21" s="6" t="s">
+      <c r="BH21" s="6" t="s">
         <v>778</v>
       </c>
-      <c r="BB21" s="3" t="s">
+      <c r="BJ21" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B22" s="113" t="s">
+    <row r="22" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B22" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -5852,33 +6233,45 @@
       <c r="AN22" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP22" s="40" t="s">
+      <c r="AP22" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="AQ22" s="6" t="s">
+        <v>942</v>
+      </c>
+      <c r="AR22" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS22" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX22" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AQ22" s="41"/>
-      <c r="AR22" s="41"/>
-      <c r="AS22" s="42"/>
-      <c r="AU22" s="3" t="s">
+      <c r="AY22" s="45"/>
+      <c r="AZ22" s="45"/>
+      <c r="BA22" s="46"/>
+      <c r="BC22" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="AW22" s="3" t="s">
+      <c r="BE22" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="AX22" s="6" t="s">
+      <c r="BF22" s="6" t="s">
         <v>766</v>
       </c>
-      <c r="AY22" s="6" t="s">
+      <c r="BG22" s="6" t="s">
         <v>773</v>
       </c>
-      <c r="AZ22" s="6" t="s">
+      <c r="BH22" s="6" t="s">
         <v>787</v>
       </c>
-      <c r="BB22" s="3" t="s">
+      <c r="BJ22" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="113" t="s">
+    <row r="23" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -5952,33 +6345,45 @@
       <c r="AN23" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP23" s="40" t="s">
+      <c r="AP23" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="AQ23" s="6" t="s">
+        <v>943</v>
+      </c>
+      <c r="AR23" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS23" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX23" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="AQ23" s="41"/>
-      <c r="AR23" s="41"/>
-      <c r="AS23" s="42"/>
-      <c r="AU23" s="8" t="s">
+      <c r="AY23" s="45"/>
+      <c r="AZ23" s="45"/>
+      <c r="BA23" s="46"/>
+      <c r="BC23" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="AW23" s="3" t="s">
+      <c r="BE23" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="AX23" s="6" t="s">
+      <c r="BF23" s="6" t="s">
         <v>767</v>
       </c>
-      <c r="AY23" s="6" t="s">
+      <c r="BG23" s="6" t="s">
         <v>773</v>
       </c>
-      <c r="AZ23" s="3" t="s">
+      <c r="BH23" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="BB23" s="8" t="s">
+      <c r="BJ23" s="8" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="113" t="s">
+    <row r="24" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -6044,27 +6449,39 @@
       <c r="AN24" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AP24" s="64" t="s">
+      <c r="AP24" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="AQ24" s="6" t="s">
+        <v>944</v>
+      </c>
+      <c r="AR24" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS24" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="AX24" s="64" t="s">
         <v>311</v>
       </c>
-      <c r="AQ24" s="65"/>
-      <c r="AR24" s="65"/>
-      <c r="AS24" s="66"/>
-      <c r="AW24" s="4" t="s">
+      <c r="AY24" s="65"/>
+      <c r="AZ24" s="65"/>
+      <c r="BA24" s="66"/>
+      <c r="BE24" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="AX24" s="8" t="s">
+      <c r="BF24" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="AY24" s="8" t="s">
+      <c r="BG24" s="8" t="s">
         <v>773</v>
       </c>
-      <c r="AZ24" s="4" t="s">
+      <c r="BH24" s="4" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="25" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="113" t="s">
+    <row r="25" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="41" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -6086,7 +6503,7 @@
       <c r="I25" s="6" t="s">
         <v>845</v>
       </c>
-      <c r="J25" s="111">
+      <c r="J25" s="39">
         <v>0</v>
       </c>
       <c r="L25" s="3"/>
@@ -6142,15 +6559,27 @@
       <c r="AN25" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AW25" s="43" t="s">
+      <c r="AP25" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="AQ25" s="6" t="s">
+        <v>945</v>
+      </c>
+      <c r="AR25" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS25" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BE25" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="AX25" s="44"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="45"/>
-    </row>
-    <row r="26" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="113" t="s">
+      <c r="BF25" s="50"/>
+      <c r="BG25" s="50"/>
+      <c r="BH25" s="51"/>
+    </row>
+    <row r="26" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -6220,15 +6649,27 @@
       <c r="AN26" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AW26" s="46" t="s">
+      <c r="AP26" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="AQ26" s="6" t="s">
+        <v>946</v>
+      </c>
+      <c r="AR26" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS26" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BE26" s="52" t="s">
         <v>315</v>
       </c>
-      <c r="AX26" s="47"/>
-      <c r="AY26" s="47"/>
-      <c r="AZ26" s="48"/>
-    </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B27" s="113" t="s">
+      <c r="BF26" s="53"/>
+      <c r="BG26" s="53"/>
+      <c r="BH26" s="54"/>
+    </row>
+    <row r="27" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B27" s="41" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -6314,14 +6755,26 @@
       <c r="AN27" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AV27" s="1"/>
-      <c r="AW27" s="1"/>
-      <c r="AX27" s="1"/>
-      <c r="AY27" s="1"/>
-      <c r="AZ27" s="1"/>
-    </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B28" s="113" t="s">
+      <c r="AP27" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="AQ27" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="AR27" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS27" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BD27" s="1"/>
+      <c r="BE27" s="1"/>
+      <c r="BF27" s="1"/>
+      <c r="BG27" s="1"/>
+      <c r="BH27" s="1"/>
+    </row>
+    <row r="28" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B28" s="41" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -6411,14 +6864,26 @@
       <c r="AN28" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AV28" s="1"/>
-      <c r="AW28" s="1"/>
-      <c r="AX28" s="1"/>
-      <c r="AY28" s="1"/>
-      <c r="AZ28" s="1"/>
-    </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B29" s="113" t="s">
+      <c r="AP28" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="AQ28" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="AR28" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS28" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+    </row>
+    <row r="29" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B29" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -6508,12 +6973,24 @@
       <c r="AN29" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AV29" s="1"/>
-      <c r="AW29" s="1"/>
-      <c r="AX29" s="1"/>
-    </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B30" s="113"/>
+      <c r="AP29" s="6" t="s">
+        <v>925</v>
+      </c>
+      <c r="AQ29" s="6" t="s">
+        <v>925</v>
+      </c>
+      <c r="AR29" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS29" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BD29" s="1"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
+    </row>
+    <row r="30" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B30" s="41"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -6579,12 +7056,24 @@
       <c r="AN30" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="AV30" s="1"/>
-      <c r="AW30" s="1"/>
-      <c r="AX30" s="1"/>
-    </row>
-    <row r="31" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="113" t="s">
+      <c r="AP30" s="6" t="s">
+        <v>926</v>
+      </c>
+      <c r="AQ30" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="AR30" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS30" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="BD30" s="1"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
+    </row>
+    <row r="31" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="41" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="3"/>
@@ -6668,14 +7157,26 @@
       <c r="AN31" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="s">
+      <c r="AP31" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AQ31" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="AR31" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="AS31" s="6" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="32" spans="2:62" x14ac:dyDescent="0.25">
+      <c r="B32" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="51"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="74"/>
       <c r="F32" s="1"/>
       <c r="G32" s="55"/>
       <c r="H32" s="56"/>
@@ -6738,12 +7239,24 @@
       <c r="AN32" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="33" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B33" s="114"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="116"/>
+      <c r="AP32" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="AQ32" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="AR32" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="AS32" s="6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="33" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="82"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="84"/>
       <c r="F33" s="1"/>
       <c r="G33" s="58" t="s">
         <v>29</v>
@@ -6810,12 +7323,24 @@
       <c r="AN33" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="34" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B34" s="114"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="116"/>
+      <c r="AP33" s="8" t="s">
+        <v>928</v>
+      </c>
+      <c r="AQ33" s="8" t="s">
+        <v>951</v>
+      </c>
+      <c r="AR33" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="AS33" s="8" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="34" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B34" s="82"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="84"/>
       <c r="F34" s="1"/>
       <c r="G34" s="58"/>
       <c r="H34" s="59"/>
@@ -6878,12 +7403,18 @@
       <c r="AN34" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="35" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="52"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
+      <c r="AP34" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="AQ34" s="45"/>
+      <c r="AR34" s="45"/>
+      <c r="AS34" s="46"/>
+    </row>
+    <row r="35" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="75"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="77"/>
       <c r="F35" s="1"/>
       <c r="G35" s="61" t="s">
         <v>32</v>
@@ -6950,8 +7481,14 @@
       <c r="AN35" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="36" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="AP35" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ35" s="45"/>
+      <c r="AR35" s="45"/>
+      <c r="AS35" s="46"/>
+    </row>
+    <row r="36" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
       <c r="D36" s="59"/>
@@ -7004,8 +7541,14 @@
       <c r="AN36" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="37" spans="2:40" x14ac:dyDescent="0.25">
+      <c r="AP36" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ36" s="45"/>
+      <c r="AR36" s="45"/>
+      <c r="AS36" s="46"/>
+    </row>
+    <row r="37" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V37" s="3" t="s">
         <v>63</v>
       </c>
@@ -7054,8 +7597,14 @@
       <c r="AN37" s="6" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="38" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP37" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ37" s="65"/>
+      <c r="AR37" s="65"/>
+      <c r="AS37" s="66"/>
+    </row>
+    <row r="38" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V38" s="3" t="s">
         <v>65</v>
       </c>
@@ -7105,7 +7654,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V39" s="3" t="s">
         <v>66</v>
       </c>
@@ -7130,12 +7679,12 @@
       <c r="AD39" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="AF39" s="68" t="s">
+      <c r="AF39" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="AG39" s="69"/>
-      <c r="AH39" s="69"/>
-      <c r="AI39" s="70"/>
+      <c r="AG39" s="68"/>
+      <c r="AH39" s="68"/>
+      <c r="AI39" s="69"/>
       <c r="AK39" s="3" t="s">
         <v>268</v>
       </c>
@@ -7149,7 +7698,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="40" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V40" s="3" t="s">
         <v>67</v>
       </c>
@@ -7174,12 +7723,12 @@
       <c r="AD40" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="AF40" s="40" t="s">
+      <c r="AF40" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AG40" s="41"/>
-      <c r="AH40" s="41"/>
-      <c r="AI40" s="42"/>
+      <c r="AG40" s="45"/>
+      <c r="AH40" s="45"/>
+      <c r="AI40" s="46"/>
       <c r="AK40" s="3" t="s">
         <v>269</v>
       </c>
@@ -7193,7 +7742,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="41" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V41" s="3" t="s">
         <v>69</v>
       </c>
@@ -7218,12 +7767,12 @@
       <c r="AD41" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="AF41" s="40" t="s">
+      <c r="AF41" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AG41" s="41"/>
-      <c r="AH41" s="41"/>
-      <c r="AI41" s="42"/>
+      <c r="AG41" s="45"/>
+      <c r="AH41" s="45"/>
+      <c r="AI41" s="46"/>
       <c r="AK41" s="3" t="s">
         <v>270</v>
       </c>
@@ -7237,7 +7786,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="42" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V42" s="3" t="s">
         <v>68</v>
       </c>
@@ -7281,7 +7830,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="43" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V43" s="3" t="s">
         <v>70</v>
       </c>
@@ -7319,7 +7868,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="44" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V44" s="3" t="s">
         <v>71</v>
       </c>
@@ -7357,7 +7906,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="45" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V45" s="3" t="s">
         <v>72</v>
       </c>
@@ -7395,7 +7944,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="46" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V46" s="3" t="s">
         <v>73</v>
       </c>
@@ -7433,7 +7982,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="47" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V47" s="3" t="s">
         <v>74</v>
       </c>
@@ -7471,7 +8020,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="48" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:45" x14ac:dyDescent="0.25">
       <c r="V48" s="3" t="s">
         <v>75</v>
       </c>
@@ -7509,7 +8058,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="49" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="49" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V49" s="3" t="s">
         <v>76</v>
       </c>
@@ -7547,7 +8096,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="50" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="50" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V50" s="3" t="s">
         <v>77</v>
       </c>
@@ -7585,7 +8134,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="51" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="51" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V51" s="3" t="s">
         <v>78</v>
       </c>
@@ -7623,7 +8172,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="52" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V52" s="3" t="s">
         <v>79</v>
       </c>
@@ -7661,7 +8210,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="53" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="53" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V53" s="3" t="s">
         <v>80</v>
       </c>
@@ -7699,7 +8248,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="54" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="54" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V54" s="3" t="s">
         <v>81</v>
       </c>
@@ -7737,7 +8286,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="55" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="55" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V55" s="3" t="s">
         <v>82</v>
       </c>
@@ -7775,7 +8324,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="56" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V56" s="3" t="s">
         <v>83</v>
       </c>
@@ -7812,8 +8361,12 @@
       <c r="AN56" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="57" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP56" s="1"/>
+      <c r="AQ56" s="23"/>
+      <c r="AR56" s="23"/>
+      <c r="AS56" s="23"/>
+    </row>
+    <row r="57" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V57" s="3" t="s">
         <v>84</v>
       </c>
@@ -7850,8 +8403,12 @@
       <c r="AN57" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="58" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP57" s="1"/>
+      <c r="AQ57" s="23"/>
+      <c r="AR57" s="23"/>
+      <c r="AS57" s="23"/>
+    </row>
+    <row r="58" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V58" s="3" t="s">
         <v>472</v>
       </c>
@@ -7888,8 +8445,12 @@
       <c r="AN58" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="59" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP58" s="1"/>
+      <c r="AQ58" s="23"/>
+      <c r="AR58" s="23"/>
+      <c r="AS58" s="23"/>
+    </row>
+    <row r="59" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V59" s="3" t="s">
         <v>85</v>
       </c>
@@ -7926,8 +8487,12 @@
       <c r="AN59" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="60" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP59" s="23"/>
+      <c r="AQ59" s="23"/>
+      <c r="AR59" s="23"/>
+      <c r="AS59" s="43"/>
+    </row>
+    <row r="60" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V60" s="3" t="s">
         <v>86</v>
       </c>
@@ -7964,8 +8529,12 @@
       <c r="AN60" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="61" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="23"/>
+      <c r="AR60" s="23"/>
+      <c r="AS60" s="23"/>
+    </row>
+    <row r="61" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V61" s="3" t="s">
         <v>87</v>
       </c>
@@ -8002,8 +8571,12 @@
       <c r="AN61" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="62" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="23"/>
+      <c r="AR61" s="23"/>
+      <c r="AS61" s="23"/>
+    </row>
+    <row r="62" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V62" s="3" t="s">
         <v>88</v>
       </c>
@@ -8040,8 +8613,12 @@
       <c r="AN62" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="63" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP62" s="1"/>
+      <c r="AQ62" s="23"/>
+      <c r="AR62" s="23"/>
+      <c r="AS62" s="23"/>
+    </row>
+    <row r="63" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V63" s="3" t="s">
         <v>89</v>
       </c>
@@ -8078,8 +8655,12 @@
       <c r="AN63" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="64" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP63" s="23"/>
+      <c r="AQ63" s="23"/>
+      <c r="AR63" s="23"/>
+      <c r="AS63" s="23"/>
+    </row>
+    <row r="64" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V64" s="3" t="s">
         <v>90</v>
       </c>
@@ -8116,8 +8697,12 @@
       <c r="AN64" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="65" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP64" s="23"/>
+      <c r="AQ64" s="23"/>
+      <c r="AR64" s="23"/>
+      <c r="AS64" s="23"/>
+    </row>
+    <row r="65" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V65" s="3" t="s">
         <v>91</v>
       </c>
@@ -8154,8 +8739,12 @@
       <c r="AN65" s="6" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="66" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AP65" s="23"/>
+      <c r="AQ65" s="23"/>
+      <c r="AR65" s="23"/>
+      <c r="AS65" s="23"/>
+    </row>
+    <row r="66" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V66" s="3" t="s">
         <v>92</v>
       </c>
@@ -8193,7 +8782,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="67" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="67" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V67" s="3" t="s">
         <v>93</v>
       </c>
@@ -8231,7 +8820,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="68" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="68" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V68" s="3" t="s">
         <v>94</v>
       </c>
@@ -8269,7 +8858,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="69" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="69" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V69" s="3" t="s">
         <v>95</v>
       </c>
@@ -8307,7 +8896,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="70" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="70" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V70" s="3" t="s">
         <v>96</v>
       </c>
@@ -8345,7 +8934,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="71" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="71" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V71" s="3" t="s">
         <v>97</v>
       </c>
@@ -8383,7 +8972,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="72" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="72" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V72" s="3" t="s">
         <v>98</v>
       </c>
@@ -8421,7 +9010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="73" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V73" s="3" t="s">
         <v>99</v>
       </c>
@@ -8459,7 +9048,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="74" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="74" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V74" s="3" t="s">
         <v>100</v>
       </c>
@@ -8497,7 +9086,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="75" spans="22:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="22:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V75" s="3" t="s">
         <v>101</v>
       </c>
@@ -8535,7 +9124,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="76" spans="22:40" x14ac:dyDescent="0.25">
+    <row r="76" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V76" s="3" t="s">
         <v>102</v>
       </c>
@@ -8560,14 +9149,14 @@
       <c r="AD76" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="AK76" s="68" t="s">
+      <c r="AK76" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="AL76" s="69"/>
-      <c r="AM76" s="69"/>
-      <c r="AN76" s="70"/>
-    </row>
-    <row r="77" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AL76" s="68"/>
+      <c r="AM76" s="68"/>
+      <c r="AN76" s="69"/>
+    </row>
+    <row r="77" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V77" s="3" t="s">
         <v>103</v>
       </c>
@@ -8592,14 +9181,14 @@
       <c r="AD77" s="18">
         <v>0</v>
       </c>
-      <c r="AK77" s="40" t="s">
+      <c r="AK77" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AL77" s="41"/>
-      <c r="AM77" s="41"/>
-      <c r="AN77" s="42"/>
-    </row>
-    <row r="78" spans="22:40" x14ac:dyDescent="0.25">
+      <c r="AL77" s="45"/>
+      <c r="AM77" s="45"/>
+      <c r="AN77" s="46"/>
+    </row>
+    <row r="78" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V78" s="3" t="s">
         <v>104</v>
       </c>
@@ -8624,14 +9213,14 @@
       <c r="AD78" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="AK78" s="40" t="s">
+      <c r="AK78" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AL78" s="41"/>
-      <c r="AM78" s="41"/>
-      <c r="AN78" s="42"/>
-    </row>
-    <row r="79" spans="22:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL78" s="45"/>
+      <c r="AM78" s="45"/>
+      <c r="AN78" s="46"/>
+    </row>
+    <row r="79" spans="22:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V79" s="3" t="s">
         <v>128</v>
       </c>
@@ -8663,7 +9252,7 @@
       <c r="AM79" s="65"/>
       <c r="AN79" s="66"/>
     </row>
-    <row r="80" spans="22:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="22:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V80" s="3" t="s">
         <v>105</v>
       </c>
@@ -8702,12 +9291,12 @@
       <c r="Y81" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AA81" s="68" t="s">
+      <c r="AA81" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="AB81" s="69"/>
-      <c r="AC81" s="69"/>
-      <c r="AD81" s="70"/>
+      <c r="AB81" s="68"/>
+      <c r="AC81" s="68"/>
+      <c r="AD81" s="69"/>
     </row>
     <row r="82" spans="22:37" x14ac:dyDescent="0.25">
       <c r="V82" s="3" t="s">
@@ -8722,12 +9311,12 @@
       <c r="Y82" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AA82" s="40" t="s">
+      <c r="AA82" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AB82" s="41"/>
-      <c r="AC82" s="41"/>
-      <c r="AD82" s="42"/>
+      <c r="AB82" s="45"/>
+      <c r="AC82" s="45"/>
+      <c r="AD82" s="46"/>
     </row>
     <row r="83" spans="22:37" x14ac:dyDescent="0.25">
       <c r="V83" s="3" t="s">
@@ -8742,12 +9331,12 @@
       <c r="Y83" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="AA83" s="40" t="s">
+      <c r="AA83" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AB83" s="41"/>
-      <c r="AC83" s="41"/>
-      <c r="AD83" s="42"/>
+      <c r="AB83" s="45"/>
+      <c r="AC83" s="45"/>
+      <c r="AD83" s="46"/>
     </row>
     <row r="84" spans="22:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V84" s="3" t="s">
@@ -9256,28 +9845,28 @@
       </c>
     </row>
     <row r="119" spans="22:25" x14ac:dyDescent="0.25">
-      <c r="V119" s="68" t="s">
+      <c r="V119" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="W119" s="69"/>
-      <c r="X119" s="69"/>
-      <c r="Y119" s="70"/>
+      <c r="W119" s="68"/>
+      <c r="X119" s="68"/>
+      <c r="Y119" s="69"/>
     </row>
     <row r="120" spans="22:25" x14ac:dyDescent="0.25">
-      <c r="V120" s="40" t="s">
+      <c r="V120" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="W120" s="41"/>
-      <c r="X120" s="41"/>
-      <c r="Y120" s="42"/>
+      <c r="W120" s="45"/>
+      <c r="X120" s="45"/>
+      <c r="Y120" s="46"/>
     </row>
     <row r="121" spans="22:25" x14ac:dyDescent="0.25">
-      <c r="V121" s="40" t="s">
+      <c r="V121" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="W121" s="41"/>
-      <c r="X121" s="41"/>
-      <c r="Y121" s="42"/>
+      <c r="W121" s="45"/>
+      <c r="X121" s="45"/>
+      <c r="Y121" s="46"/>
     </row>
     <row r="122" spans="22:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V122" s="64" t="s">
@@ -9287,42 +9876,68 @@
       <c r="X122" s="65"/>
       <c r="Y122" s="66"/>
     </row>
+    <row r="128" spans="22:25" x14ac:dyDescent="0.25">
+      <c r="V128" t="s">
+        <v>893</v>
+      </c>
+      <c r="W128" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="129" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V129" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="130" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V130" t="s">
+        <v>896</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="91">
+  <mergeCells count="100">
+    <mergeCell ref="AP34:AS34"/>
+    <mergeCell ref="AP35:AS35"/>
+    <mergeCell ref="AP36:AS36"/>
+    <mergeCell ref="AP37:AS37"/>
+    <mergeCell ref="AP4:AS4"/>
+    <mergeCell ref="AP6:AP7"/>
+    <mergeCell ref="AQ6:AQ7"/>
+    <mergeCell ref="AR6:AR7"/>
+    <mergeCell ref="AS6:AS7"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="B32:E35"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="G33:J33"/>
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="G35:J35"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="L34:O34"/>
     <mergeCell ref="L35:O35"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="AX6:AX7"/>
-    <mergeCell ref="AY6:AY7"/>
-    <mergeCell ref="AZ6:AZ7"/>
-    <mergeCell ref="AW4:AZ4"/>
+    <mergeCell ref="BF6:BF7"/>
+    <mergeCell ref="AX17:BA17"/>
+    <mergeCell ref="AX18:BA18"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="BG6:BG7"/>
+    <mergeCell ref="BH6:BH7"/>
+    <mergeCell ref="BE4:BH4"/>
     <mergeCell ref="L32:O32"/>
     <mergeCell ref="B4:T4"/>
     <mergeCell ref="AL6:AL7"/>
     <mergeCell ref="AM6:AM7"/>
     <mergeCell ref="AN6:AN7"/>
-    <mergeCell ref="AS6:AS7"/>
-    <mergeCell ref="AP4:AS4"/>
-    <mergeCell ref="AQ6:AQ7"/>
-    <mergeCell ref="AR6:AR7"/>
-    <mergeCell ref="AP19:AS19"/>
-    <mergeCell ref="AP20:AS20"/>
-    <mergeCell ref="AP21:AS21"/>
-    <mergeCell ref="AP16:AS16"/>
-    <mergeCell ref="AP17:AS17"/>
-    <mergeCell ref="AP18:AS18"/>
+    <mergeCell ref="BA6:BA7"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="AY6:AY7"/>
+    <mergeCell ref="AZ6:AZ7"/>
+    <mergeCell ref="AX19:BA19"/>
+    <mergeCell ref="AX20:BA20"/>
+    <mergeCell ref="AX21:BA21"/>
+    <mergeCell ref="AX16:BA16"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="AK76:AN76"/>
     <mergeCell ref="AF39:AI39"/>
@@ -9330,20 +9945,30 @@
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="AA6:AA7"/>
     <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="AF4:AI4"/>
+    <mergeCell ref="AF40:AI40"/>
+    <mergeCell ref="AF41:AI41"/>
+    <mergeCell ref="AF42:AI42"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="X6:X7"/>
     <mergeCell ref="W6:W7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="AA4:AD4"/>
-    <mergeCell ref="AF4:AI4"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="Q6:T7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="V122:Y122"/>
-    <mergeCell ref="BB6:BB7"/>
-    <mergeCell ref="AW6:AW7"/>
-    <mergeCell ref="AP6:AP7"/>
-    <mergeCell ref="AU6:AU7"/>
+    <mergeCell ref="BJ6:BJ7"/>
+    <mergeCell ref="BE6:BE7"/>
+    <mergeCell ref="AX6:AX7"/>
+    <mergeCell ref="BC6:BC7"/>
     <mergeCell ref="V119:Y119"/>
     <mergeCell ref="AB6:AB7"/>
     <mergeCell ref="AC6:AC7"/>
@@ -9355,15 +9980,12 @@
     <mergeCell ref="AG6:AG7"/>
     <mergeCell ref="AH6:AH7"/>
     <mergeCell ref="AI6:AI7"/>
-    <mergeCell ref="AF40:AI40"/>
-    <mergeCell ref="AF41:AI41"/>
-    <mergeCell ref="AF42:AI42"/>
     <mergeCell ref="V120:Y120"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="V121:Y121"/>
-    <mergeCell ref="AW25:AZ25"/>
-    <mergeCell ref="AW26:AZ26"/>
+    <mergeCell ref="BE25:BH25"/>
+    <mergeCell ref="BE26:BH26"/>
     <mergeCell ref="Q15:T15"/>
     <mergeCell ref="Q16:T16"/>
     <mergeCell ref="Q17:T17"/>
@@ -9371,15 +9993,9 @@
     <mergeCell ref="AK77:AN77"/>
     <mergeCell ref="AK78:AN78"/>
     <mergeCell ref="AK79:AN79"/>
-    <mergeCell ref="AP22:AS22"/>
-    <mergeCell ref="AP23:AS23"/>
-    <mergeCell ref="AP24:AS24"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q6:T7"/>
+    <mergeCell ref="AX22:BA22"/>
+    <mergeCell ref="AX23:BA23"/>
+    <mergeCell ref="AX24:BA24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9391,14 +10007,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F76CB4-6E73-48BB-89E3-7365BCD76DEB}">
   <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
@@ -9407,11 +10023,11 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="52" t="s">
         <v>465</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
       <c r="F2" s="17" t="s">
         <v>493</v>
       </c>
@@ -9424,18 +10040,18 @@
       <c r="L2" s="17" t="s">
         <v>711</v>
       </c>
-      <c r="N2" s="82" t="s">
+      <c r="N2" s="91" t="s">
         <v>797</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="84"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="116" t="s">
         <v>474</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="109"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="118"/>
       <c r="F3" s="14" t="s">
         <v>474</v>
       </c>
@@ -9448,18 +10064,18 @@
       <c r="L3" s="36" t="s">
         <v>712</v>
       </c>
-      <c r="N3" s="85" t="s">
+      <c r="N3" s="94" t="s">
         <v>796</v>
       </c>
-      <c r="O3" s="86"/>
-      <c r="P3" s="87"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="107" t="s">
         <v>451</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="100"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="109"/>
       <c r="F4" s="15" t="s">
         <v>494</v>
       </c>
@@ -9472,18 +10088,18 @@
       <c r="L4" s="27" t="s">
         <v>713</v>
       </c>
-      <c r="N4" s="91" t="s">
+      <c r="N4" s="100" t="s">
         <v>451</v>
       </c>
-      <c r="O4" s="92"/>
-      <c r="P4" s="93"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="102"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="107" t="s">
         <v>452</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="100"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
       <c r="F5" s="15" t="s">
         <v>495</v>
       </c>
@@ -9496,18 +10112,18 @@
       <c r="L5" s="27" t="s">
         <v>714</v>
       </c>
-      <c r="N5" s="91" t="s">
+      <c r="N5" s="100" t="s">
         <v>452</v>
       </c>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="102"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="107" t="s">
         <v>453</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="109"/>
       <c r="F6" s="15" t="s">
         <v>496</v>
       </c>
@@ -9520,18 +10136,18 @@
       <c r="L6" s="27" t="s">
         <v>715</v>
       </c>
-      <c r="N6" s="91" t="s">
+      <c r="N6" s="100" t="s">
         <v>453</v>
       </c>
-      <c r="O6" s="92"/>
-      <c r="P6" s="93"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="102"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="107" t="s">
         <v>454</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="100"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="109"/>
       <c r="F7" s="15" t="s">
         <v>497</v>
       </c>
@@ -9544,18 +10160,18 @@
       <c r="L7" s="27" t="s">
         <v>716</v>
       </c>
-      <c r="N7" s="91" t="s">
+      <c r="N7" s="100" t="s">
         <v>454</v>
       </c>
-      <c r="O7" s="92"/>
-      <c r="P7" s="93"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="102"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="107" t="s">
         <v>455</v>
       </c>
-      <c r="C8" s="99"/>
-      <c r="D8" s="100"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="109"/>
       <c r="F8" s="15" t="s">
         <v>211</v>
       </c>
@@ -9568,18 +10184,18 @@
       <c r="L8" s="27" t="s">
         <v>717</v>
       </c>
-      <c r="N8" s="91" t="s">
+      <c r="N8" s="100" t="s">
         <v>455</v>
       </c>
-      <c r="O8" s="92"/>
-      <c r="P8" s="93"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="102"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="107" t="s">
         <v>456</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="100"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="109"/>
       <c r="F9" s="15" t="s">
         <v>498</v>
       </c>
@@ -9592,18 +10208,18 @@
       <c r="L9" s="27" t="s">
         <v>718</v>
       </c>
-      <c r="N9" s="91" t="s">
+      <c r="N9" s="100" t="s">
         <v>456</v>
       </c>
-      <c r="O9" s="92"/>
-      <c r="P9" s="93"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="102"/>
     </row>
     <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="107" t="s">
         <v>457</v>
       </c>
-      <c r="C10" s="99"/>
-      <c r="D10" s="100"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="109"/>
       <c r="F10" s="15" t="s">
         <v>499</v>
       </c>
@@ -9616,18 +10232,18 @@
       <c r="L10" s="27" t="s">
         <v>719</v>
       </c>
-      <c r="N10" s="91" t="s">
+      <c r="N10" s="100" t="s">
         <v>457</v>
       </c>
-      <c r="O10" s="92"/>
-      <c r="P10" s="93"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="102"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="107" t="s">
         <v>458</v>
       </c>
-      <c r="C11" s="99"/>
-      <c r="D11" s="100"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="109"/>
       <c r="F11" s="15" t="s">
         <v>500</v>
       </c>
@@ -9637,48 +10253,48 @@
       <c r="L11" s="28" t="s">
         <v>720</v>
       </c>
-      <c r="N11" s="91" t="s">
+      <c r="N11" s="100" t="s">
         <v>458</v>
       </c>
-      <c r="O11" s="92"/>
-      <c r="P11" s="93"/>
+      <c r="O11" s="101"/>
+      <c r="P11" s="102"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="107" t="s">
         <v>459</v>
       </c>
-      <c r="C12" s="99"/>
-      <c r="D12" s="100"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
       <c r="F12" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="N12" s="91" t="s">
+      <c r="N12" s="100" t="s">
         <v>459</v>
       </c>
-      <c r="O12" s="92"/>
-      <c r="P12" s="93"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="102"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="107" t="s">
         <v>460</v>
       </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="100"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="109"/>
       <c r="F13" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="N13" s="91" t="s">
+      <c r="N13" s="100" t="s">
         <v>460</v>
       </c>
-      <c r="O13" s="92"/>
-      <c r="P13" s="93"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="102"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="107" t="s">
         <v>461</v>
       </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="100"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="109"/>
       <c r="F14" s="15" t="s">
         <v>502</v>
       </c>
@@ -9691,18 +10307,18 @@
       <c r="L14" s="9" t="s">
         <v>779</v>
       </c>
-      <c r="N14" s="91" t="s">
+      <c r="N14" s="100" t="s">
         <v>461</v>
       </c>
-      <c r="O14" s="92"/>
-      <c r="P14" s="93"/>
+      <c r="O14" s="101"/>
+      <c r="P14" s="102"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="107" t="s">
         <v>462</v>
       </c>
-      <c r="C15" s="99"/>
-      <c r="D15" s="100"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
       <c r="F15" s="16" t="s">
         <v>503</v>
       </c>
@@ -9715,18 +10331,18 @@
       <c r="L15" s="14" t="s">
         <v>781</v>
       </c>
-      <c r="N15" s="91" t="s">
+      <c r="N15" s="100" t="s">
         <v>462</v>
       </c>
-      <c r="O15" s="92"/>
-      <c r="P15" s="93"/>
+      <c r="O15" s="101"/>
+      <c r="P15" s="102"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="107" t="s">
         <v>463</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="100"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="109"/>
       <c r="H16" s="15" t="s">
         <v>592</v>
       </c>
@@ -9736,18 +10352,18 @@
       <c r="L16" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="N16" s="91" t="s">
+      <c r="N16" s="100" t="s">
         <v>463</v>
       </c>
-      <c r="O16" s="92"/>
-      <c r="P16" s="93"/>
+      <c r="O16" s="101"/>
+      <c r="P16" s="102"/>
     </row>
     <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="110" t="s">
         <v>464</v>
       </c>
-      <c r="C17" s="102"/>
-      <c r="D17" s="103"/>
+      <c r="C17" s="111"/>
+      <c r="D17" s="112"/>
       <c r="H17" s="20" t="s">
         <v>593</v>
       </c>
@@ -9757,16 +10373,16 @@
       <c r="L17" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="N17" s="94" t="s">
+      <c r="N17" s="103" t="s">
         <v>464</v>
       </c>
-      <c r="O17" s="95"/>
-      <c r="P17" s="96"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="105"/>
     </row>
     <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
       <c r="H18" s="16" t="s">
         <v>594</v>
       </c>
@@ -9776,9 +10392,9 @@
       <c r="L18" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="N18" s="97"/>
-      <c r="O18" s="97"/>
-      <c r="P18" s="97"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="106"/>
     </row>
     <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
@@ -9788,18 +10404,18 @@
       <c r="L19" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="N19" s="88" t="s">
+      <c r="N19" s="97" t="s">
         <v>801</v>
       </c>
-      <c r="O19" s="89"/>
-      <c r="P19" s="89"/>
-      <c r="Q19" s="90"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="99"/>
     </row>
     <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="105" t="s">
+      <c r="B20" s="114" t="s">
         <v>485</v>
       </c>
-      <c r="C20" s="106"/>
+      <c r="C20" s="115"/>
       <c r="F20" s="9" t="s">
         <v>595</v>
       </c>
@@ -9809,18 +10425,18 @@
       <c r="L20" s="6" t="s">
         <v>786</v>
       </c>
-      <c r="N20" s="85" t="s">
+      <c r="N20" s="94" t="s">
         <v>796</v>
       </c>
-      <c r="O20" s="86"/>
-      <c r="P20" s="86"/>
-      <c r="Q20" s="87"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="96"/>
     </row>
     <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="94" t="s">
         <v>474</v>
       </c>
-      <c r="C21" s="87"/>
+      <c r="C21" s="96"/>
       <c r="F21" s="14" t="s">
         <v>596</v>
       </c>
@@ -9831,18 +10447,18 @@
         <v>703</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="N21" s="76" t="s">
+      <c r="N21" s="85" t="s">
         <v>802</v>
       </c>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="78"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="87"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="85" t="s">
         <v>479</v>
       </c>
-      <c r="C22" s="78"/>
+      <c r="C22" s="87"/>
       <c r="F22" s="18" t="s">
         <v>597</v>
       </c>
@@ -9852,18 +10468,18 @@
       <c r="J22" s="25" t="s">
         <v>704</v>
       </c>
-      <c r="N22" s="76" t="s">
+      <c r="N22" s="85" t="s">
         <v>803</v>
       </c>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="78"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="86"/>
+      <c r="Q22" s="87"/>
     </row>
     <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="85" t="s">
         <v>480</v>
       </c>
-      <c r="C23" s="78"/>
+      <c r="C23" s="87"/>
       <c r="F23" s="18" t="s">
         <v>598</v>
       </c>
@@ -9873,78 +10489,78 @@
       <c r="J23" s="26" t="s">
         <v>705</v>
       </c>
-      <c r="N23" s="76" t="s">
+      <c r="N23" s="85" t="s">
         <v>804</v>
       </c>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="78"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="87"/>
     </row>
     <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="85" t="s">
         <v>481</v>
       </c>
-      <c r="C24" s="78"/>
+      <c r="C24" s="87"/>
       <c r="F24" s="21" t="s">
         <v>599</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>606</v>
       </c>
-      <c r="N24" s="76" t="s">
+      <c r="N24" s="85" t="s">
         <v>805</v>
       </c>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="78"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="87"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="85" t="s">
         <v>482</v>
       </c>
-      <c r="C25" s="78"/>
+      <c r="C25" s="87"/>
       <c r="H25" s="15" t="s">
         <v>607</v>
       </c>
-      <c r="N25" s="76" t="s">
+      <c r="N25" s="85" t="s">
         <v>806</v>
       </c>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="78"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="86"/>
+      <c r="Q25" s="87"/>
     </row>
     <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="85" t="s">
         <v>483</v>
       </c>
-      <c r="C26" s="78"/>
+      <c r="C26" s="87"/>
       <c r="H26" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="N26" s="76" t="s">
+      <c r="N26" s="85" t="s">
         <v>807</v>
       </c>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="78"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="86"/>
+      <c r="Q26" s="87"/>
     </row>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="88" t="s">
         <v>484</v>
       </c>
-      <c r="C27" s="81"/>
+      <c r="C27" s="90"/>
       <c r="H27" s="15" t="s">
         <v>609</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>729</v>
       </c>
-      <c r="N27" s="76" t="s">
+      <c r="N27" s="85" t="s">
         <v>808</v>
       </c>
-      <c r="O27" s="77"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="78"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="87"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
@@ -9954,12 +10570,12 @@
       <c r="J28" s="14" t="s">
         <v>796</v>
       </c>
-      <c r="N28" s="76" t="s">
+      <c r="N28" s="85" t="s">
         <v>809</v>
       </c>
-      <c r="O28" s="77"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="78"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="87"/>
     </row>
     <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
@@ -9969,12 +10585,12 @@
       <c r="J29" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="N29" s="76" t="s">
+      <c r="N29" s="85" t="s">
         <v>810</v>
       </c>
-      <c r="O29" s="77"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="78"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="87"/>
     </row>
     <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
@@ -9987,100 +10603,130 @@
       <c r="L30" s="9" t="s">
         <v>785</v>
       </c>
-      <c r="N30" s="76" t="s">
+      <c r="N30" s="85" t="s">
         <v>811</v>
       </c>
-      <c r="O30" s="77"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="78"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O30" s="86"/>
+      <c r="P30" s="86"/>
+      <c r="Q30" s="87"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
       <c r="J31" s="15" t="s">
         <v>726</v>
       </c>
       <c r="L31" s="2"/>
-      <c r="N31" s="76" t="s">
+      <c r="N31" s="85" t="s">
         <v>812</v>
       </c>
-      <c r="O31" s="77"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="78"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O31" s="86"/>
+      <c r="P31" s="86"/>
+      <c r="Q31" s="87"/>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
+      <c r="D32" s="42" t="s">
+        <v>897</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>901</v>
+      </c>
       <c r="J32" s="29" t="s">
         <v>727</v>
       </c>
       <c r="L32" s="31">
         <v>180000</v>
       </c>
-      <c r="N32" s="76" t="s">
+      <c r="N32" s="85" t="s">
         <v>813</v>
       </c>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="78"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="86"/>
+      <c r="Q32" s="87"/>
     </row>
     <row r="33" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
+      <c r="D33" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="J33" s="16" t="s">
         <v>728</v>
       </c>
       <c r="L33" s="31">
         <v>90000</v>
       </c>
-      <c r="N33" s="76" t="s">
+      <c r="N33" s="85" t="s">
         <v>814</v>
       </c>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="78"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="86"/>
+      <c r="Q33" s="87"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
+      <c r="D34" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>898</v>
+      </c>
       <c r="L34" s="31">
         <v>60000</v>
       </c>
-      <c r="N34" s="76" t="s">
+      <c r="N34" s="85" t="s">
         <v>815</v>
       </c>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="78"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="86"/>
+      <c r="Q34" s="87"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
+      <c r="D35" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>900</v>
+      </c>
       <c r="L35" s="31">
         <v>30000</v>
       </c>
-      <c r="N35" s="76" t="s">
+      <c r="N35" s="85" t="s">
         <v>816</v>
       </c>
-      <c r="O35" s="77"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="78"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="87"/>
     </row>
     <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
+      <c r="D36" s="4" t="s">
+        <v>899</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>899</v>
+      </c>
       <c r="L36" s="33" t="s">
         <v>792</v>
       </c>
-      <c r="N36" s="76" t="s">
+      <c r="N36" s="85" t="s">
         <v>817</v>
       </c>
-      <c r="O36" s="77"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="78"/>
+      <c r="O36" s="86"/>
+      <c r="P36" s="86"/>
+      <c r="Q36" s="87"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13"/>
-      <c r="N37" s="79" t="s">
+      <c r="N37" s="88" t="s">
         <v>818</v>
       </c>
-      <c r="O37" s="80"/>
-      <c r="P37" s="80"/>
-      <c r="Q37" s="81"/>
+      <c r="O37" s="89"/>
+      <c r="P37" s="89"/>
+      <c r="Q37" s="90"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>

</xml_diff>